<commit_message>
fixed hp search for other metrics
</commit_message>
<xml_diff>
--- a/results_experiments/timings/timings_inference.xlsx
+++ b/results_experiments/timings/timings_inference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Elias\hover_next_train\results_experiments\timings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A522E4-1070-489D-8A36-996AC145E932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CD9D01-E5C3-4FA9-83ED-E6145FC6A967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-75720" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="33">
   <si>
     <t>ncores</t>
   </si>
@@ -127,6 +127,15 @@
   <si>
     <t>XEON E5-2630 v8</t>
   </si>
+  <si>
+    <t>pannuke</t>
+  </si>
+  <si>
+    <t>hovernet</t>
+  </si>
+  <si>
+    <t>OOM</t>
+  </si>
 </sst>
 </file>
 
@@ -167,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -449,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2019,6 +2029,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H56" s="1">
+        <v>0.56680555555555556</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H58" s="1"/>
+    </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>25</v>
@@ -2777,6 +2798,706 @@
       </c>
       <c r="L83">
         <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>4</v>
+      </c>
+      <c r="D91">
+        <v>32</v>
+      </c>
+      <c r="E91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91" t="s">
+        <v>21</v>
+      </c>
+      <c r="I91" t="s">
+        <v>15</v>
+      </c>
+      <c r="J91">
+        <v>58</v>
+      </c>
+      <c r="K91">
+        <v>4</v>
+      </c>
+      <c r="L91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>4</v>
+      </c>
+      <c r="D92">
+        <v>32</v>
+      </c>
+      <c r="E92" t="s">
+        <v>30</v>
+      </c>
+      <c r="F92" t="s">
+        <v>5</v>
+      </c>
+      <c r="G92">
+        <v>4</v>
+      </c>
+      <c r="H92" t="s">
+        <v>21</v>
+      </c>
+      <c r="I92" t="s">
+        <v>16</v>
+      </c>
+      <c r="J92">
+        <v>127</v>
+      </c>
+      <c r="K92">
+        <v>4</v>
+      </c>
+      <c r="L92" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93">
+        <v>4</v>
+      </c>
+      <c r="D93">
+        <v>32</v>
+      </c>
+      <c r="E93" t="s">
+        <v>30</v>
+      </c>
+      <c r="F93" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93">
+        <v>4</v>
+      </c>
+      <c r="H93" t="s">
+        <v>21</v>
+      </c>
+      <c r="I93" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93">
+        <v>235</v>
+      </c>
+      <c r="K93">
+        <v>4</v>
+      </c>
+      <c r="L93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>32</v>
+      </c>
+      <c r="E94" t="s">
+        <v>30</v>
+      </c>
+      <c r="F94" t="s">
+        <v>5</v>
+      </c>
+      <c r="G94">
+        <v>4</v>
+      </c>
+      <c r="H94" t="s">
+        <v>21</v>
+      </c>
+      <c r="I94" t="s">
+        <v>18</v>
+      </c>
+      <c r="J94">
+        <v>391</v>
+      </c>
+      <c r="K94">
+        <v>4</v>
+      </c>
+      <c r="L94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95">
+        <v>4</v>
+      </c>
+      <c r="D95">
+        <v>32</v>
+      </c>
+      <c r="E95" t="s">
+        <v>30</v>
+      </c>
+      <c r="F95" t="s">
+        <v>5</v>
+      </c>
+      <c r="G95">
+        <v>4</v>
+      </c>
+      <c r="H95" t="s">
+        <v>21</v>
+      </c>
+      <c r="I95" t="s">
+        <v>12</v>
+      </c>
+      <c r="J95">
+        <v>1017</v>
+      </c>
+      <c r="K95">
+        <v>4</v>
+      </c>
+      <c r="L95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>25</v>
+      </c>
+      <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96">
+        <v>20</v>
+      </c>
+      <c r="D96">
+        <v>128</v>
+      </c>
+      <c r="E96" t="s">
+        <v>30</v>
+      </c>
+      <c r="F96" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" t="s">
+        <v>14</v>
+      </c>
+      <c r="H96" t="s">
+        <v>22</v>
+      </c>
+      <c r="I96" t="s">
+        <v>15</v>
+      </c>
+      <c r="J96">
+        <v>56</v>
+      </c>
+      <c r="K96">
+        <v>20</v>
+      </c>
+      <c r="L96">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97">
+        <v>20</v>
+      </c>
+      <c r="D97">
+        <v>128</v>
+      </c>
+      <c r="E97" t="s">
+        <v>30</v>
+      </c>
+      <c r="F97" t="s">
+        <v>14</v>
+      </c>
+      <c r="G97" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" t="s">
+        <v>22</v>
+      </c>
+      <c r="I97" t="s">
+        <v>16</v>
+      </c>
+      <c r="J97">
+        <v>108</v>
+      </c>
+      <c r="K97">
+        <v>20</v>
+      </c>
+      <c r="L97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>27</v>
+      </c>
+      <c r="B98" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98">
+        <v>20</v>
+      </c>
+      <c r="D98">
+        <v>128</v>
+      </c>
+      <c r="E98" t="s">
+        <v>30</v>
+      </c>
+      <c r="F98" t="s">
+        <v>14</v>
+      </c>
+      <c r="G98" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98" t="s">
+        <v>22</v>
+      </c>
+      <c r="I98" t="s">
+        <v>17</v>
+      </c>
+      <c r="J98">
+        <v>200</v>
+      </c>
+      <c r="K98">
+        <v>20</v>
+      </c>
+      <c r="L98">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99">
+        <v>20</v>
+      </c>
+      <c r="D99">
+        <v>128</v>
+      </c>
+      <c r="E99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F99" t="s">
+        <v>14</v>
+      </c>
+      <c r="G99" t="s">
+        <v>14</v>
+      </c>
+      <c r="H99" t="s">
+        <v>22</v>
+      </c>
+      <c r="I99" t="s">
+        <v>18</v>
+      </c>
+      <c r="J99">
+        <v>263</v>
+      </c>
+      <c r="K99">
+        <v>20</v>
+      </c>
+      <c r="L99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>29</v>
+      </c>
+      <c r="B100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100">
+        <v>20</v>
+      </c>
+      <c r="D100">
+        <v>128</v>
+      </c>
+      <c r="E100" t="s">
+        <v>30</v>
+      </c>
+      <c r="F100" t="s">
+        <v>14</v>
+      </c>
+      <c r="G100" t="s">
+        <v>14</v>
+      </c>
+      <c r="H100" t="s">
+        <v>22</v>
+      </c>
+      <c r="I100" t="s">
+        <v>12</v>
+      </c>
+      <c r="J100">
+        <v>542</v>
+      </c>
+      <c r="K100">
+        <v>20</v>
+      </c>
+      <c r="L100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B103" t="s">
+        <v>11</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103">
+        <v>128</v>
+      </c>
+      <c r="E103" t="s">
+        <v>30</v>
+      </c>
+      <c r="F103" t="s">
+        <v>31</v>
+      </c>
+      <c r="G103" t="s">
+        <v>14</v>
+      </c>
+      <c r="H103" t="s">
+        <v>21</v>
+      </c>
+      <c r="I103" t="s">
+        <v>15</v>
+      </c>
+      <c r="J103">
+        <v>6643</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <v>128</v>
+      </c>
+      <c r="E104" t="s">
+        <v>30</v>
+      </c>
+      <c r="F104" t="s">
+        <v>31</v>
+      </c>
+      <c r="G104" t="s">
+        <v>14</v>
+      </c>
+      <c r="H104" t="s">
+        <v>21</v>
+      </c>
+      <c r="I104" t="s">
+        <v>16</v>
+      </c>
+      <c r="J104" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>128</v>
+      </c>
+      <c r="E105" t="s">
+        <v>30</v>
+      </c>
+      <c r="F105" t="s">
+        <v>31</v>
+      </c>
+      <c r="G105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" t="s">
+        <v>21</v>
+      </c>
+      <c r="I105" t="s">
+        <v>17</v>
+      </c>
+      <c r="J105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>9</v>
+      </c>
+      <c r="B106" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>128</v>
+      </c>
+      <c r="E106" t="s">
+        <v>30</v>
+      </c>
+      <c r="F106" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" t="s">
+        <v>21</v>
+      </c>
+      <c r="I106" t="s">
+        <v>18</v>
+      </c>
+      <c r="J106" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107">
+        <v>4</v>
+      </c>
+      <c r="D107">
+        <v>128</v>
+      </c>
+      <c r="E107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" t="s">
+        <v>31</v>
+      </c>
+      <c r="G107" t="s">
+        <v>14</v>
+      </c>
+      <c r="H107" t="s">
+        <v>21</v>
+      </c>
+      <c r="I107" t="s">
+        <v>12</v>
+      </c>
+      <c r="J107" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108">
+        <v>128</v>
+      </c>
+      <c r="E108" t="s">
+        <v>30</v>
+      </c>
+      <c r="F108" t="s">
+        <v>31</v>
+      </c>
+      <c r="G108" t="s">
+        <v>14</v>
+      </c>
+      <c r="H108" t="s">
+        <v>22</v>
+      </c>
+      <c r="I108" t="s">
+        <v>15</v>
+      </c>
+      <c r="J108">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>9</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>4</v>
+      </c>
+      <c r="D109">
+        <v>128</v>
+      </c>
+      <c r="E109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F109" t="s">
+        <v>31</v>
+      </c>
+      <c r="G109" t="s">
+        <v>14</v>
+      </c>
+      <c r="H109" t="s">
+        <v>22</v>
+      </c>
+      <c r="I109" t="s">
+        <v>16</v>
+      </c>
+      <c r="J109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+      <c r="D110">
+        <v>128</v>
+      </c>
+      <c r="E110" t="s">
+        <v>30</v>
+      </c>
+      <c r="F110" t="s">
+        <v>31</v>
+      </c>
+      <c r="G110" t="s">
+        <v>14</v>
+      </c>
+      <c r="H110" t="s">
+        <v>22</v>
+      </c>
+      <c r="I110" t="s">
+        <v>17</v>
+      </c>
+      <c r="J110" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111">
+        <v>4</v>
+      </c>
+      <c r="D111">
+        <v>128</v>
+      </c>
+      <c r="E111" t="s">
+        <v>30</v>
+      </c>
+      <c r="F111" t="s">
+        <v>31</v>
+      </c>
+      <c r="G111" t="s">
+        <v>14</v>
+      </c>
+      <c r="H111" t="s">
+        <v>22</v>
+      </c>
+      <c r="I111" t="s">
+        <v>18</v>
+      </c>
+      <c r="J111" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112">
+        <v>4</v>
+      </c>
+      <c r="D112">
+        <v>128</v>
+      </c>
+      <c r="E112" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112" t="s">
+        <v>31</v>
+      </c>
+      <c r="G112" t="s">
+        <v>14</v>
+      </c>
+      <c r="H112" t="s">
+        <v>22</v>
+      </c>
+      <c r="I112" t="s">
+        <v>12</v>
+      </c>
+      <c r="J112" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>